<commit_message>
dj added comments to excel file
</commit_message>
<xml_diff>
--- a/Lab1/MissingValue_Replacment_Puri.xlsx
+++ b/Lab1/MissingValue_Replacment_Puri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/puri/DataScience@SMU/06.DS7331 ML1/Team Project/airbnb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OaklandHillsMansion\Desktop\SMUGitHub\DS7731MachineLearning\airbnb\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{724CB4E0-97A6-314D-AACE-61D00164D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F1216-3F77-4B3A-94E8-2C502F28A283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76800" yWindow="-5780" windowWidth="38400" windowHeight="21100" xr2:uid="{7DBAEDCC-443D-7B45-B2A5-16E2E09FA79A}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{7DBAEDCC-443D-7B45-B2A5-16E2E09FA79A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>minimum_minimum_nights</t>
   </si>
@@ -127,6 +118,27 @@
   </si>
   <si>
     <t>Column</t>
+  </si>
+  <si>
+    <t>bathrooms</t>
+  </si>
+  <si>
+    <t>bathroom_text</t>
+  </si>
+  <si>
+    <t>beds</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Turned text string to float and saved float values in "bathroom" colummn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used cleaned values from bathroom text column, used mean for null values, outliers seemed reasonable </t>
+  </si>
+  <si>
+    <t>Kept it simple and used mean, ouliers seemed reasonable</t>
   </si>
 </sst>
 </file>
@@ -551,20 +563,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C18356-00E3-FB49-A575-F8D5580A2F98}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="85.1640625" customWidth="1"/>
+    <col min="3" max="3" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -575,108 +587,106 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -685,9 +695,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -696,9 +706,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -707,9 +717,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -718,58 +728,91 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>